<commit_message>
Add: google doc API and added PDF generation script
</commit_message>
<xml_diff>
--- a/crypto_data.xlsx
+++ b/crypto_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,31 +469,11 @@
           <t>24h Price Change (%)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Top 5 by Market Cap</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Average Price (Top 50)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Highest 24h Change (%)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Lowest 24h Change (%)</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -507,40 +487,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>97031.77267598263</v>
+        <v>96951.96523877764</v>
       </c>
       <c r="E2" t="n">
-        <v>1923436571812.835</v>
+        <v>1921854568936.979</v>
       </c>
       <c r="F2" t="n">
-        <v>30417818832.48621</v>
+        <v>32047027088.08397</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.35911864</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.04005806</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -554,40 +516,22 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2663.73502963684</v>
+        <v>2657.458581349047</v>
       </c>
       <c r="E3" t="n">
-        <v>321088521027.2768</v>
+        <v>320331953472.4678</v>
       </c>
       <c r="F3" t="n">
-        <v>17576670517.2694</v>
+        <v>18233536635.77166</v>
       </c>
       <c r="G3" t="n">
-        <v>0.39543057</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.2469151</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -601,40 +545,22 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2.471707651201206</v>
+        <v>2.469977247227968</v>
       </c>
       <c r="E4" t="n">
-        <v>142772126053.2659</v>
+        <v>142672173514.7567</v>
       </c>
       <c r="F4" t="n">
-        <v>4546186191.864518</v>
+        <v>4529294831.526029</v>
       </c>
       <c r="G4" t="n">
-        <v>1.61354092</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.07258177</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -648,40 +574,22 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.000363878194604</v>
+        <v>1.000027167131255</v>
       </c>
       <c r="E5" t="n">
-        <v>141931137689.1731</v>
+        <v>141883365288.2145</v>
       </c>
       <c r="F5" t="n">
-        <v>75262917089.3822</v>
+        <v>76095565589.54431</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01345386</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.02252833</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -695,40 +603,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>199.9132876151964</v>
+        <v>199.7853531921762</v>
       </c>
       <c r="E6" t="n">
-        <v>97572642453.96199</v>
+        <v>97510200883.09988</v>
       </c>
       <c r="F6" t="n">
-        <v>3873219857.050404</v>
+        <v>3815448138.406306</v>
       </c>
       <c r="G6" t="n">
-        <v>-2.31837629</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-1.35989756</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -742,40 +632,22 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>637.3329027012547</v>
+        <v>637.2252607176524</v>
       </c>
       <c r="E7" t="n">
-        <v>90806854337.0229</v>
+        <v>90791517564.22475</v>
       </c>
       <c r="F7" t="n">
-        <v>2098892242.973405</v>
+        <v>2096870271.034158</v>
       </c>
       <c r="G7" t="n">
-        <v>5.5990731</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>5.41538713</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -789,40 +661,22 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.000444461532643</v>
+        <v>1.000021873452921</v>
       </c>
       <c r="E8" t="n">
-        <v>56438628526.61394</v>
+        <v>56414788830.7905</v>
       </c>
       <c r="F8" t="n">
-        <v>6702511063.87799</v>
+        <v>6728429306.624347</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03937809</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.00263601</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -836,40 +690,22 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.2602495184953756</v>
+        <v>0.2592114313494296</v>
       </c>
       <c r="E9" t="n">
-        <v>38517588829.95361</v>
+        <v>38363949299.36627</v>
       </c>
       <c r="F9" t="n">
-        <v>1524017872.487675</v>
+        <v>1529096728.560311</v>
       </c>
       <c r="G9" t="n">
-        <v>3.38875452</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>3.23526021</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -883,40 +719,22 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7948109015906903</v>
+        <v>0.7955866463901666</v>
       </c>
       <c r="E10" t="n">
-        <v>27975120516.344</v>
+        <v>28002424563.39701</v>
       </c>
       <c r="F10" t="n">
-        <v>1530157966.507305</v>
+        <v>1530365619.688709</v>
       </c>
       <c r="G10" t="n">
-        <v>12.8879898</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>13.79743441</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -930,40 +748,22 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.2452082441340159</v>
+        <v>0.245097540632702</v>
       </c>
       <c r="E11" t="n">
-        <v>21113354146.68189</v>
+        <v>21103822157.91547</v>
       </c>
       <c r="F11" t="n">
-        <v>630664987.2536405</v>
+        <v>629768210.6461357</v>
       </c>
       <c r="G11" t="n">
-        <v>2.73921613</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.74940672</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -977,40 +777,22 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>19.21656311874533</v>
+        <v>19.13697028282434</v>
       </c>
       <c r="E12" t="n">
-        <v>12262088358.27551</v>
+        <v>12211300172.02607</v>
       </c>
       <c r="F12" t="n">
-        <v>437716969.6412452</v>
+        <v>435531259.850859</v>
       </c>
       <c r="G12" t="n">
-        <v>2.94478515</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.81074856</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1024,40 +806,22 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>26.23412375728378</v>
+        <v>26.16969941800279</v>
       </c>
       <c r="E13" t="n">
-        <v>10805678177.13549</v>
+        <v>10779142178.31634</v>
       </c>
       <c r="F13" t="n">
-        <v>330681856.3097058</v>
+        <v>329663263.4409063</v>
       </c>
       <c r="G13" t="n">
-        <v>3.10454662</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.83414465</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1071,40 +835,22 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.483059191433017</v>
+        <v>3.469153193794336</v>
       </c>
       <c r="E14" t="n">
-        <v>10761633042.6709</v>
+        <v>10718667581.71985</v>
       </c>
       <c r="F14" t="n">
-        <v>1286876214.5428</v>
+        <v>1278758947.436697</v>
       </c>
       <c r="G14" t="n">
-        <v>6.60264499</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>7.01699561</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1118,40 +864,22 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.3327018519003066</v>
+        <v>0.3317166307125556</v>
       </c>
       <c r="E15" t="n">
-        <v>10176335378.26307</v>
+        <v>10146200465.66472</v>
       </c>
       <c r="F15" t="n">
-        <v>360708014.3959396</v>
+        <v>360431862.1137937</v>
       </c>
       <c r="G15" t="n">
-        <v>5.54358037</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>5.52200819</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1165,40 +893,22 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>126.629851246962</v>
+        <v>126.273526251122</v>
       </c>
       <c r="E16" t="n">
-        <v>9563258842.877275</v>
+        <v>9536348693.857521</v>
       </c>
       <c r="F16" t="n">
-        <v>1922337053.34847</v>
+        <v>1918753408.29971</v>
       </c>
       <c r="G16" t="n">
-        <v>6.98308729</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>6.92145967</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1212,40 +922,22 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3.787854557449477</v>
+        <v>3.782175849886186</v>
       </c>
       <c r="E17" t="n">
-        <v>9446977067.744164</v>
+        <v>9432814269.434149</v>
       </c>
       <c r="F17" t="n">
-        <v>118111313.1546824</v>
+        <v>117936521.7087271</v>
       </c>
       <c r="G17" t="n">
-        <v>0.08930861</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.15349725</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1259,134 +951,80 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1.588036493649582e-05</v>
+        <v>1.592349244967839e-05</v>
       </c>
       <c r="E18" t="n">
-        <v>9357566985.911741</v>
+        <v>9382980041.288963</v>
       </c>
       <c r="F18" t="n">
-        <v>252299799.2559999</v>
+        <v>254741992.4694594</v>
       </c>
       <c r="G18" t="n">
-        <v>0.35132326</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.8045837300000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>UNUS SED LEO</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>LEO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.2381989339250491</v>
+        <v>9.821772419149164</v>
       </c>
       <c r="E19" t="n">
-        <v>9115283229.708254</v>
+        <v>9076735506.8039</v>
       </c>
       <c r="F19" t="n">
-        <v>300097996.3204784</v>
+        <v>680361.07955605</v>
       </c>
       <c r="G19" t="n">
-        <v>0.87396854</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.34693819</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UNUS SED LEO</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>LEO</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>9.827796462330356</v>
+        <v>0.2371216602003209</v>
       </c>
       <c r="E20" t="n">
-        <v>9082302592.2854</v>
+        <v>9074058632.456654</v>
       </c>
       <c r="F20" t="n">
-        <v>679836.57628979</v>
+        <v>299069737.7736334</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.25906338</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.93407922</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1400,40 +1038,22 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>24.28189217960635</v>
+        <v>24.42002475488977</v>
       </c>
       <c r="E21" t="n">
-        <v>8108408062.492181</v>
+        <v>8154534421.955286</v>
       </c>
       <c r="F21" t="n">
-        <v>109595093.3735659</v>
+        <v>111085583.9685851</v>
       </c>
       <c r="G21" t="n">
-        <v>1.28276865</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.95271855</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1447,40 +1067,22 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5.000972261634724</v>
+        <v>4.982182232981482</v>
       </c>
       <c r="E22" t="n">
-        <v>7739140825.19757</v>
+        <v>7710062743.926749</v>
       </c>
       <c r="F22" t="n">
-        <v>238072984.670756</v>
+        <v>237495225.621421</v>
       </c>
       <c r="G22" t="n">
-        <v>3.40324813</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>3.06105358</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1494,40 +1096,22 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>6.388573707895687</v>
+        <v>6.386980939373784</v>
       </c>
       <c r="E23" t="n">
-        <v>7666288449.474824</v>
+        <v>7664377127.24854</v>
       </c>
       <c r="F23" t="n">
-        <v>217267645.8776272</v>
+        <v>217159426.5944348</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.85227825</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.97039484</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1541,40 +1125,22 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>338.1876375507785</v>
+        <v>337.355458257882</v>
       </c>
       <c r="E24" t="n">
-        <v>6705570738.48406</v>
+        <v>6689070321.271792</v>
       </c>
       <c r="F24" t="n">
-        <v>222551768.7959689</v>
+        <v>223779752.197539</v>
       </c>
       <c r="G24" t="n">
-        <v>2.63234073</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.4117663</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1588,134 +1154,80 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.000563766776237</v>
+        <v>1.000381203188641</v>
       </c>
       <c r="E25" t="n">
-        <v>6044002516.027678</v>
+        <v>6042899722.963003</v>
       </c>
       <c r="F25" t="n">
-        <v>161921762.2409994</v>
+        <v>161623292.6697673</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0506871</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.04069769</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Uniswap</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>9.731462090506962</v>
+        <v>6.020892442108516</v>
       </c>
       <c r="E26" t="n">
-        <v>5843918518.640496</v>
+        <v>5827563228.893959</v>
       </c>
       <c r="F26" t="n">
-        <v>243943175.7439006</v>
+        <v>185188424.1548026</v>
       </c>
       <c r="G26" t="n">
-        <v>5.55489632</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I26" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-1.00292944</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>Uniswap</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OM</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>6.030393455296855</v>
+        <v>9.6317183337642</v>
       </c>
       <c r="E27" t="n">
-        <v>5836759167.141647</v>
+        <v>5784020593.567509</v>
       </c>
       <c r="F27" t="n">
-        <v>186225076.0499917</v>
+        <v>249096049.9268193</v>
       </c>
       <c r="G27" t="n">
-        <v>-1.17145081</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>4.52663874</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1729,40 +1241,22 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1.000142961635893</v>
+        <v>0.999908843561119</v>
       </c>
       <c r="E28" t="n">
-        <v>5366149746.55324</v>
+        <v>5364893613.484464</v>
       </c>
       <c r="F28" t="n">
-        <v>202108463.7985026</v>
+        <v>202352987.9299155</v>
       </c>
       <c r="G28" t="n">
-        <v>0.00476434</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I28" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.03967516</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1776,40 +1270,22 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1.415343377659195</v>
+        <v>1.402241525630146</v>
       </c>
       <c r="E29" t="n">
-        <v>4471221920.483454</v>
+        <v>4429831761.09464</v>
       </c>
       <c r="F29" t="n">
-        <v>395944878.1388668</v>
+        <v>398094580.1057393</v>
       </c>
       <c r="G29" t="n">
-        <v>5.0807216</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I29" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>4.58002861</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1823,40 +1299,22 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1.001840455634668e-05</v>
+        <v>9.98743690559449e-06</v>
       </c>
       <c r="E30" t="n">
-        <v>4214641610.968978</v>
+        <v>4201613833.070804</v>
       </c>
       <c r="F30" t="n">
-        <v>846507521.6936538</v>
+        <v>844402354.5868996</v>
       </c>
       <c r="G30" t="n">
-        <v>4.11704494</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I30" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>4.15123345</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1870,40 +1328,22 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>222.8739978636615</v>
+        <v>221.8092651397445</v>
       </c>
       <c r="E31" t="n">
-        <v>4111299599.275454</v>
+        <v>4091658747.210453</v>
       </c>
       <c r="F31" t="n">
-        <v>74287646.83916971</v>
+        <v>74132438.55104646</v>
       </c>
       <c r="G31" t="n">
-        <v>0.4971419</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I31" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-0.25616641</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1917,40 +1357,22 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.331093159653962</v>
+        <v>3.32071646040998</v>
       </c>
       <c r="E32" t="n">
-        <v>3943274555.179047</v>
+        <v>3930990847.658904</v>
       </c>
       <c r="F32" t="n">
-        <v>192241381.1905822</v>
+        <v>190585491.318728</v>
       </c>
       <c r="G32" t="n">
-        <v>3.65563367</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>3.50285276</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1964,40 +1386,22 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>251.431858165647</v>
+        <v>250.5473993526707</v>
       </c>
       <c r="E33" t="n">
-        <v>3788440492.096981</v>
+        <v>3775113940.700044</v>
       </c>
       <c r="F33" t="n">
-        <v>339180246.8746588</v>
+        <v>336595138.7023382</v>
       </c>
       <c r="G33" t="n">
-        <v>0.94532981</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.86287241</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2011,40 +1415,22 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.039338443487465</v>
+        <v>1.041826512502634</v>
       </c>
       <c r="E34" t="n">
-        <v>3497056222.668659</v>
+        <v>3505427814.508108</v>
       </c>
       <c r="F34" t="n">
-        <v>133404226.3296851</v>
+        <v>133213523.3163068</v>
       </c>
       <c r="G34" t="n">
-        <v>1.9749827</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.41339102</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2058,40 +1444,22 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>7.253677401741902</v>
+        <v>7.22542472433302</v>
       </c>
       <c r="E35" t="n">
-        <v>3485758628.816193</v>
+        <v>3472181789.289042</v>
       </c>
       <c r="F35" t="n">
-        <v>99359199.54651731</v>
+        <v>98760877.12858939</v>
       </c>
       <c r="G35" t="n">
-        <v>2.63339251</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.56334432</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2105,40 +1473,22 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>421.0140124447856</v>
+        <v>420.2889743574618</v>
       </c>
       <c r="E36" t="n">
-        <v>3458727787.484801</v>
+        <v>3452771431.3886</v>
       </c>
       <c r="F36" t="n">
-        <v>232268011.0125125</v>
+        <v>229940930.6816522</v>
       </c>
       <c r="G36" t="n">
-        <v>7.62822435</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>8.50916104</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2152,40 +1502,22 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>5.970028708709018</v>
+        <v>5.965794011222634</v>
       </c>
       <c r="E37" t="n">
-        <v>3432508080.239733</v>
+        <v>3430073312.494281</v>
       </c>
       <c r="F37" t="n">
-        <v>263259436.8507233</v>
+        <v>261925259.8610212</v>
       </c>
       <c r="G37" t="n">
-        <v>-4.20011002</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I37" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-3.50209603</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2199,40 +1531,22 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>15.79799500376107</v>
+        <v>15.79218850647863</v>
       </c>
       <c r="E38" t="n">
-        <v>3159593014.198296</v>
+        <v>3158431716.942146</v>
       </c>
       <c r="F38" t="n">
-        <v>919386997.9215711</v>
+        <v>910125461.4900885</v>
       </c>
       <c r="G38" t="n">
-        <v>-1.10556665</v>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I38" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-1.39140174</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2246,40 +1560,22 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>20.84453556939762</v>
+        <v>20.79367542696373</v>
       </c>
       <c r="E39" t="n">
-        <v>3141471703.627227</v>
+        <v>3133806591.695776</v>
       </c>
       <c r="F39" t="n">
-        <v>129103668.433271</v>
+        <v>128658395.4559813</v>
       </c>
       <c r="G39" t="n">
-        <v>1.56983625</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>1.42714961</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2293,40 +1589,22 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>51.34169176877935</v>
+        <v>51.16114276198959</v>
       </c>
       <c r="E40" t="n">
-        <v>3080501506.126761</v>
+        <v>3069668565.719375</v>
       </c>
       <c r="F40" t="n">
-        <v>7791930.38885975</v>
+        <v>7796388.75959986</v>
       </c>
       <c r="G40" t="n">
-        <v>6.96438319</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I40" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>7.05202354</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2340,40 +1618,22 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.03428631545422554</v>
+        <v>0.03420527131217486</v>
       </c>
       <c r="E41" t="n">
-        <v>2776678668.868067</v>
+        <v>2770115305.686938</v>
       </c>
       <c r="F41" t="n">
-        <v>53522984.53954312</v>
+        <v>53463193.30723769</v>
       </c>
       <c r="G41" t="n">
-        <v>2.80296913</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.86922896</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2387,40 +1647,22 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.3150728064403456</v>
+        <v>0.3144724195911433</v>
       </c>
       <c r="E42" t="n">
-        <v>2696789617.64268</v>
+        <v>2691650751.360342</v>
       </c>
       <c r="F42" t="n">
-        <v>112489503.0580871</v>
+        <v>112467501.9905337</v>
       </c>
       <c r="G42" t="n">
-        <v>2.5525642</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.83643899</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2434,40 +1676,22 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.1008761252113042</v>
+        <v>0.1005561387819687</v>
       </c>
       <c r="E43" t="n">
-        <v>2592352156.300583</v>
+        <v>2584140312.955206</v>
       </c>
       <c r="F43" t="n">
-        <v>109193059.2072705</v>
+        <v>109032825.9415184</v>
       </c>
       <c r="G43" t="n">
-        <v>11.00621011</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I43" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>11.61602133</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2481,40 +1705,22 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.09465976144514454</v>
+        <v>0.09441704483410708</v>
       </c>
       <c r="E44" t="n">
-        <v>2515257596.708539</v>
+        <v>2508808237.54643</v>
       </c>
       <c r="F44" t="n">
-        <v>18275827.20376543</v>
+        <v>18333156.55417059</v>
       </c>
       <c r="G44" t="n">
-        <v>1.27854378</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I44" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>1.1989765</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2528,40 +1734,22 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.2983117772595285</v>
+        <v>0.2974259714222846</v>
       </c>
       <c r="E45" t="n">
-        <v>2513497439.951149</v>
+        <v>2506033870.37753</v>
       </c>
       <c r="F45" t="n">
-        <v>130054783.0892306</v>
+        <v>129210486.7186098</v>
       </c>
       <c r="G45" t="n">
-        <v>2.95895041</v>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>3.26140972</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2575,40 +1763,22 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4.642281823528032</v>
+        <v>4.626781032009151</v>
       </c>
       <c r="E46" t="n">
-        <v>2403386315.757195</v>
+        <v>2395361298.828866</v>
       </c>
       <c r="F46" t="n">
-        <v>67141653.11860558</v>
+        <v>67262734.51100573</v>
       </c>
       <c r="G46" t="n">
-        <v>5.22463848</v>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I46" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>5.01793081</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2622,40 +1792,22 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.8364714340272968</v>
+        <v>0.8348667579423246</v>
       </c>
       <c r="E47" t="n">
-        <v>2206142289.549179</v>
+        <v>2201910054.438601</v>
       </c>
       <c r="F47" t="n">
-        <v>164360774.8778421</v>
+        <v>172391841.9991602</v>
       </c>
       <c r="G47" t="n">
-        <v>-1.54148743</v>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I47" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>-1.17660372</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2669,40 +1821,22 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3.420674038148565</v>
+        <v>3.409952063373729</v>
       </c>
       <c r="E48" t="n">
-        <v>2151544775.231217</v>
+        <v>2144800838.641619</v>
       </c>
       <c r="F48" t="n">
-        <v>126782807.6933264</v>
+        <v>126152077.5056315</v>
       </c>
       <c r="G48" t="n">
-        <v>0.92808702</v>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>0.65783485</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2716,40 +1850,22 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.4721471824517999</v>
+        <v>0.4709347509713709</v>
       </c>
       <c r="E49" t="n">
-        <v>2050942475.271923</v>
+        <v>2045675839.540548</v>
       </c>
       <c r="F49" t="n">
-        <v>171583262.1310157</v>
+        <v>171189992.7209592</v>
       </c>
       <c r="G49" t="n">
-        <v>1.84674165</v>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>1.68950258</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2763,40 +1879,22 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>21.95300718639238</v>
+        <v>22.07497235038408</v>
       </c>
       <c r="E50" t="n">
-        <v>1948315023.444001</v>
+        <v>1959139351.943704</v>
       </c>
       <c r="F50" t="n">
-        <v>17297301.5206693</v>
+        <v>17197523.01695884</v>
       </c>
       <c r="G50" t="n">
-        <v>1.57925085</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>3.02285594</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-02-11 20:55:47</t>
+          <t>2025-02-11 21:11:34</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2810,34 +1908,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.7921177325275699</v>
+        <v>0.7923608657377742</v>
       </c>
       <c r="E51" t="n">
-        <v>1893126940.32233</v>
+        <v>1893708018.12355</v>
       </c>
       <c r="F51" t="n">
-        <v>138581290.1085113</v>
+        <v>140381200.330985</v>
       </c>
       <c r="G51" t="n">
-        <v>1.86464311</v>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Bitcoin, Ethereum, XRP, Tether USDt, Solana</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>2043.103439433483</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>12.89% (Cardano)</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>-4.20% (Aptos)</t>
-        </is>
+        <v>2.488205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>